<commit_message>
fix math foriegn key level 10
</commit_message>
<xml_diff>
--- a/Yemen -General Education -level 10.xlsx
+++ b/Yemen -General Education -level 10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Downloads\Mozakara Python Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745F8395-B4CE-45ED-9DC3-3B73D3B93E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432A8DB9-8D9E-4CF6-A34F-3665CE497EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A965D38E-D5A1-4F7D-981C-A0C2D194DFD0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A965D38E-D5A1-4F7D-981C-A0C2D194DFD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="4" r:id="rId1"/>
@@ -30881,8 +30881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDE1D5F-FA2D-4056-83FB-E71A749FB85B}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G25" activeCellId="3" sqref="G22 G23 G24 G25:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -31932,7 +31932,7 @@
         <v>5</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H22" s="1" t="b">
         <v>0</v>
@@ -31980,7 +31980,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H23" s="1" t="b">
         <v>0</v>
@@ -32028,7 +32028,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H24" s="1" t="b">
         <v>0</v>
@@ -32076,7 +32076,7 @@
         <v>5</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H25" s="1" t="b">
         <v>0</v>
@@ -32124,7 +32124,7 @@
         <v>5</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H26" s="1" t="b">
         <v>0</v>
@@ -32172,7 +32172,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H27" s="1" t="b">
         <v>0</v>
@@ -32220,7 +32220,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H28" s="1" t="b">
         <v>0</v>
@@ -32268,7 +32268,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H29" s="1" t="b">
         <v>0</v>
@@ -32316,7 +32316,7 @@
         <v>5</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H30" s="1" t="b">
         <v>0</v>
@@ -34370,8 +34370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4488DD4-EA49-4CE4-BEF9-1378EB01B3D6}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>